<commit_message>
them conkhai vao fileattachment
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/FileAttachment.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/FileAttachment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CongViec\MyProjects\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC66CD9-4DD1-43E7-9FE7-0836A87CC5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D527EEB-9F40-41B3-B0A3-181F212E9909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Nội dung chính</t>
+  </si>
+  <si>
+    <t>Hình thức:</t>
+  </si>
+  <si>
+    <t>Công khai:</t>
+  </si>
+  <si>
+    <t>Giai đoạn:</t>
   </si>
 </sst>
 </file>
@@ -488,18 +497,18 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="19.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,19 +553,25 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>

</xml_diff>

<commit_message>
fix bug file attachment
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/FileAttachment.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/FileAttachment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\KNTC\SourceCode\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797EA284-835B-4F90-BA6F-67C1B1D83F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E5331B-2CDB-4019-B793-B8567E15EABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
@@ -496,8 +496,8 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>